<commit_message>
Added November 2024 Changes
</commit_message>
<xml_diff>
--- a/schedule_2024_10.xlsx
+++ b/schedule_2024_10.xlsx
@@ -477,21 +477,21 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45572</v>
+        <v>45566</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -501,32 +501,32 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45579</v>
+        <v>45573</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -536,7 +536,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -547,21 +547,21 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45586</v>
+        <v>45580</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -571,32 +571,32 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45593</v>
+        <v>45587</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mon</t>
+          <t>Tue</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -617,7 +617,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45566</v>
+        <v>45594</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -641,18 +641,22 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
+          <t>Dr. Sharmila</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Dr. Saumya Shukla</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45573</v>
+        <v>45567</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -662,32 +666,32 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>Dr. Saumya Shukla</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Dr. Madhuri Tripathi</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Dr. Madhuri Tripathi</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Dr. Suvarna Kumar</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45580</v>
+        <v>45574</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -697,7 +701,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -707,22 +711,22 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45587</v>
+        <v>45581</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -732,7 +736,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -742,22 +746,22 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45594</v>
+        <v>45588</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tue</t>
+          <t>Wed</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -767,7 +771,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -777,18 +781,18 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45567</v>
+        <v>45595</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -812,32 +816,32 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Sharmila</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45574</v>
+        <v>45568</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -847,32 +851,32 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45581</v>
+        <v>45575</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -887,27 +891,27 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45588</v>
+        <v>45582</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -917,32 +921,32 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45595</v>
+        <v>45589</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Wed</t>
+          <t>Thu</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -952,18 +956,18 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Sharmila</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45568</v>
+        <v>45596</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -977,7 +981,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -987,32 +991,32 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45575</v>
+        <v>45569</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1022,32 +1026,32 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45582</v>
+        <v>45576</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1057,7 +1061,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1068,21 +1072,21 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45589</v>
+        <v>45583</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Sharmila</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1097,27 +1101,27 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45596</v>
+        <v>45590</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Thu</t>
+          <t>Fri</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1132,27 +1136,27 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Sharmila</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45569</v>
+        <v>45570</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Sharmila</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1162,27 +1166,27 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>Dr. Rashmi Sharma</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>Dr. Minakshi Mishra</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45576</v>
+        <v>45577</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1197,32 +1201,32 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45583</v>
+        <v>45584</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1232,32 +1236,32 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>Dr. Sharmila</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>Dr. Minakshi Mishra</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45590</v>
+        <v>45591</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Fri</t>
+          <t>Sat</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1267,27 +1271,27 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45570</v>
+        <v>45571</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1297,37 +1301,37 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Dr. Madhuri Tripathi</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Rashmi Sharma</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45577</v>
+        <v>45578</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1342,57 +1346,57 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45584</v>
+        <v>45585</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
+          <t>Dr. Madhuri Tripathi</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Dr. Madhuri Tripathi</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Dr. Minakshi Mishra</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>Dr. Sharmila</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Dr. Madhuri Tripathi</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Dr. Abhilasha Mishra</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45591</v>
+        <v>45592</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Sat</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1402,27 +1406,27 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Dr. Madhuri Tripathi</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45571</v>
+        <v>45572</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1437,42 +1441,42 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Dr. Minakshi Mishra</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45578</v>
+        <v>45579</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Dr. Madhuri Tripathi</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Suvarna Kumar</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1488,51 +1492,51 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45585</v>
+        <v>45586</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Dr. Rashmi Sharma</t>
+          <t>Dr. Amit Tripathi</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Dr. Suvarna Kumar</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Saumya Shukla</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Dr. Abhilasha Mishra</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45592</v>
+        <v>45593</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Sun</t>
+          <t>Mon</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Dr. Saumya Shukla</t>
+          <t>Dr. Abhilasha Mishra</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1542,7 +1546,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Dr. Amit Tripathi</t>
+          <t>Dr. Madhuri Tripathi</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1552,7 +1556,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Dr. Sharmila</t>
+          <t>Dr. Minakshi Mishra</t>
         </is>
       </c>
     </row>
@@ -1612,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1634,7 +1638,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="n">
         <v>4</v>
@@ -1653,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>4</v>
@@ -1666,13 +1670,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>5</v>
@@ -1688,7 +1692,7 @@
         <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -1742,13 +1746,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>

</xml_diff>